<commit_message>
fixed databases in admin page
</commit_message>
<xml_diff>
--- a/class/example.xlsx
+++ b/class/example.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
   <si>
     <t>Section</t>
   </si>
@@ -119,34 +119,40 @@
     <t>Registrar</t>
   </si>
   <si>
-    <t>A111G0001</t>
-  </si>
-  <si>
-    <t>John David Lozano</t>
-  </si>
-  <si>
-    <t>A111G0002</t>
-  </si>
-  <si>
-    <t>Jeddahlyn Cabuga</t>
-  </si>
-  <si>
-    <t>A111G0003</t>
-  </si>
-  <si>
-    <t>Janice Millanes</t>
-  </si>
-  <si>
-    <t>A111G0004</t>
-  </si>
-  <si>
-    <t>Judilyn Abcede</t>
-  </si>
-  <si>
-    <t>A111G0005</t>
-  </si>
-  <si>
-    <t>Jhansel May Conception</t>
+    <t>Mary Claire Q. Romano</t>
+  </si>
+  <si>
+    <t>Diana Jane D. Lucena</t>
+  </si>
+  <si>
+    <t>Sam J. Saracanlao</t>
+  </si>
+  <si>
+    <t>Dennis Dondon F. Serquina</t>
+  </si>
+  <si>
+    <t>Judy Dela F. Francisco</t>
+  </si>
+  <si>
+    <t>Carmela Q. Romano</t>
+  </si>
+  <si>
+    <t>A114C0440</t>
+  </si>
+  <si>
+    <t>A114C0268</t>
+  </si>
+  <si>
+    <t>A114C0269</t>
+  </si>
+  <si>
+    <t>A114C0447</t>
+  </si>
+  <si>
+    <t>A114C0426</t>
+  </si>
+  <si>
+    <t>A114C0270</t>
   </si>
 </sst>
 </file>
@@ -167,6 +173,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -348,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1">
@@ -440,6 +447,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -765,14 +775,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="3.140625" customWidth="1"/>
     <col min="11" max="11" width="2.5703125" customWidth="1"/>
     <col min="18" max="18" width="2.85546875" customWidth="1"/>
@@ -906,41 +916,41 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="36" t="s">
+      <c r="L5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
       <c r="R5" s="7"/>
-      <c r="S5" s="36" t="s">
+      <c r="S5" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="36"/>
+      <c r="T5" s="37"/>
       <c r="U5" s="7"/>
-      <c r="V5" s="36" t="s">
+      <c r="V5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="W5" s="36"/>
-      <c r="X5" s="36"/>
-      <c r="Y5" s="36"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
@@ -1013,11 +1023,11 @@
       <c r="A7" s="12">
         <v>1</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>33</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="15">
@@ -1089,10 +1099,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="24">
@@ -1129,7 +1139,7 @@
         <v>100</v>
       </c>
       <c r="P8" s="16">
-        <f t="shared" ref="P8:P11" si="2">SUM(L8:O8)/4</f>
+        <f t="shared" ref="P8:P12" si="2">SUM(L8:O8)/4</f>
         <v>100</v>
       </c>
       <c r="Q8" s="17">
@@ -1141,7 +1151,7 @@
         <v>20</v>
       </c>
       <c r="T8" s="18">
-        <f t="shared" ref="T8:T11" si="4">S8</f>
+        <f t="shared" ref="T8:T12" si="4">S8</f>
         <v>20</v>
       </c>
       <c r="U8" s="14"/>
@@ -1151,7 +1161,7 @@
       </c>
       <c r="W8" s="24"/>
       <c r="X8" s="19">
-        <f t="shared" ref="X8:X11" si="5">V8+W8</f>
+        <f t="shared" ref="X8:X12" si="5">V8+W8</f>
         <v>100</v>
       </c>
       <c r="Y8" s="21" t="str">
@@ -1163,11 +1173,11 @@
       <c r="A9" s="12">
         <v>3</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>36</v>
+      <c r="B9" s="34" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="15">
@@ -1239,10 +1249,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="24">
@@ -1305,7 +1315,7 @@
         <v>100</v>
       </c>
       <c r="Y10" s="21" t="str">
-        <f t="shared" ref="Y10:Y11" si="6">IF(X10&gt;=98,"4.0",IF(X10&gt;=94,"3.5",IF(X10&gt;=91,"3.0",IF(X10&gt;=87,"2.5",IF(X10&gt;=83,"2.0",IF(X10&gt;=79,"1.5",IF(X10&gt;=75,"1.0","Failed")))))))</f>
+        <f t="shared" ref="Y10:Y12" si="6">IF(X10&gt;=98,"4.0",IF(X10&gt;=94,"3.5",IF(X10&gt;=91,"3.0",IF(X10&gt;=87,"2.5",IF(X10&gt;=83,"2.0",IF(X10&gt;=79,"1.5",IF(X10&gt;=75,"1.0","Failed")))))))</f>
         <v>4.0</v>
       </c>
     </row>
@@ -1314,10 +1324,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="15">
@@ -1363,72 +1373,98 @@
       </c>
       <c r="R11" s="14"/>
       <c r="S11" s="24">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="T11" s="18">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="U11" s="14"/>
       <c r="V11" s="19">
         <f>J11+Q11+T11</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="W11" s="20"/>
       <c r="X11" s="19">
         <f t="shared" si="5"/>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="Y11" s="21" t="str">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>6</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
+      <c r="B12" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>37</v>
+      </c>
       <c r="D12" s="14"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
+      <c r="E12" s="24">
+        <v>100</v>
+      </c>
+      <c r="F12" s="24">
+        <v>100</v>
+      </c>
+      <c r="G12" s="24">
+        <v>100</v>
+      </c>
+      <c r="H12" s="24">
+        <v>100</v>
+      </c>
       <c r="I12" s="16">
         <f t="shared" ref="I12:I66" si="7">SUM(E12:H12)/4</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J12" s="17">
         <f t="shared" ref="J12:J66" si="8">I12*0.4</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K12" s="14"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="25">
-        <v>0</v>
+      <c r="L12" s="24">
+        <v>100</v>
+      </c>
+      <c r="M12" s="24">
+        <v>100</v>
+      </c>
+      <c r="N12" s="24">
+        <v>100</v>
+      </c>
+      <c r="O12" s="24">
+        <v>100</v>
+      </c>
+      <c r="P12" s="16">
+        <f t="shared" si="2"/>
+        <v>100</v>
       </c>
       <c r="Q12" s="26">
         <v>0</v>
       </c>
       <c r="R12" s="14"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="26">
-        <v>0</v>
+      <c r="S12" s="24">
+        <v>20</v>
+      </c>
+      <c r="T12" s="18">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="U12" s="14"/>
       <c r="V12" s="27">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="W12" s="24"/>
-      <c r="X12" s="27">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="28" t="s">
-        <v>26</v>
+      <c r="X12" s="19">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="Y12" s="21" t="str">
+        <f t="shared" si="6"/>
+        <v>4.0</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -4011,20 +4047,20 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
-      <c r="I71" s="37"/>
-      <c r="J71" s="37"/>
-      <c r="K71" s="37"/>
-      <c r="L71" s="37"/>
-      <c r="M71" s="37"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="38"/>
+      <c r="K71" s="38"/>
+      <c r="L71" s="38"/>
+      <c r="M71" s="38"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
-      <c r="R71" s="37"/>
-      <c r="S71" s="37"/>
-      <c r="T71" s="37"/>
-      <c r="U71" s="37"/>
-      <c r="V71" s="37"/>
+      <c r="R71" s="38"/>
+      <c r="S71" s="38"/>
+      <c r="T71" s="38"/>
+      <c r="U71" s="38"/>
+      <c r="V71" s="38"/>
       <c r="W71" s="29"/>
       <c r="X71" s="1"/>
       <c r="Y71" s="1"/>
@@ -4040,25 +4076,25 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
-      <c r="I72" s="34" t="s">
+      <c r="I72" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="J72" s="34"/>
-      <c r="K72" s="34"/>
-      <c r="L72" s="34"/>
-      <c r="M72" s="34"/>
+      <c r="J72" s="35"/>
+      <c r="K72" s="35"/>
+      <c r="L72" s="35"/>
+      <c r="M72" s="35"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
-      <c r="R72" s="34" t="s">
+      <c r="R72" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="S72" s="34"/>
-      <c r="T72" s="34"/>
-      <c r="U72" s="34"/>
-      <c r="V72" s="34"/>
-      <c r="W72" s="34"/>
+      <c r="S72" s="35"/>
+      <c r="T72" s="35"/>
+      <c r="U72" s="35"/>
+      <c r="V72" s="35"/>
+      <c r="W72" s="35"/>
       <c r="X72" s="1"/>
       <c r="Y72" s="1"/>
     </row>

</xml_diff>